<commit_message>
AutoFetch: update of 11/19
</commit_message>
<xml_diff>
--- a/randomStuff/AutoFetch/data/EstimateResult.xlsx
+++ b/randomStuff/AutoFetch/data/EstimateResult.xlsx
@@ -10,6 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2017-11-15" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2017-11-16" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2017-11-17" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2017-11-19" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="80">
   <si>
     <t>Date</t>
   </si>
@@ -254,6 +255,9 @@
   </si>
   <si>
     <t>ZTO</t>
+  </si>
+  <si>
+    <t>2017-11-19</t>
   </si>
 </sst>
 </file>
@@ -611,63 +615,63 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row spans="1:19" r="1">
-      <c r="B1" s="1" t="s">
+      <c s="1" r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c s="1" r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c s="1" r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c s="1" r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c s="1" r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c s="1" r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c s="1" r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c s="1" r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c s="1" r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c s="1" r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c s="1" r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c s="1" r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c s="1" r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c s="1" r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c s="1" r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c s="1" r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c s="1" r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c s="1" r="S1" t="s">
         <v>17</v>
       </c>
     </row>
     <row spans="1:19" r="2">
-      <c r="A2" s="1" t="n">
+      <c s="1" r="A2" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -726,7 +730,7 @@
       </c>
     </row>
     <row spans="1:19" r="3">
-      <c r="A3" s="1" t="n">
+      <c s="1" r="A3" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -785,7 +789,7 @@
       </c>
     </row>
     <row spans="1:19" r="4">
-      <c r="A4" s="1" t="n">
+      <c s="1" r="A4" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -844,7 +848,7 @@
       </c>
     </row>
     <row spans="1:19" r="5">
-      <c r="A5" s="1" t="n">
+      <c s="1" r="A5" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -903,7 +907,7 @@
       </c>
     </row>
     <row spans="1:19" r="6">
-      <c r="A6" s="1" t="n">
+      <c s="1" r="A6" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -962,7 +966,7 @@
       </c>
     </row>
     <row spans="1:19" r="7">
-      <c r="A7" s="1" t="n">
+      <c s="1" r="A7" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -1021,7 +1025,7 @@
       </c>
     </row>
     <row spans="1:19" r="8">
-      <c r="A8" s="1" t="n">
+      <c s="1" r="A8" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -1080,7 +1084,7 @@
       </c>
     </row>
     <row spans="1:19" r="9">
-      <c r="A9" s="1" t="n">
+      <c s="1" r="A9" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="s">
@@ -1139,7 +1143,7 @@
       </c>
     </row>
     <row spans="1:19" r="10">
-      <c r="A10" s="1" t="n">
+      <c s="1" r="A10" t="n">
         <v>8</v>
       </c>
       <c r="B10" t="s">
@@ -1198,7 +1202,7 @@
       </c>
     </row>
     <row spans="1:19" r="11">
-      <c r="A11" s="1" t="n">
+      <c s="1" r="A11" t="n">
         <v>9</v>
       </c>
       <c r="B11" t="s">
@@ -1257,7 +1261,7 @@
       </c>
     </row>
     <row spans="1:19" r="12">
-      <c r="A12" s="1" t="n">
+      <c s="1" r="A12" t="n">
         <v>10</v>
       </c>
       <c r="B12" t="s">
@@ -1316,7 +1320,7 @@
       </c>
     </row>
     <row spans="1:19" r="13">
-      <c r="A13" s="1" t="n">
+      <c s="1" r="A13" t="n">
         <v>11</v>
       </c>
       <c r="B13" t="s">
@@ -1375,7 +1379,7 @@
       </c>
     </row>
     <row spans="1:19" r="14">
-      <c r="A14" s="1" t="n">
+      <c s="1" r="A14" t="n">
         <v>12</v>
       </c>
       <c r="B14" t="s">
@@ -1434,7 +1438,7 @@
       </c>
     </row>
     <row spans="1:19" r="15">
-      <c r="A15" s="1" t="n">
+      <c s="1" r="A15" t="n">
         <v>13</v>
       </c>
       <c r="B15" t="s">
@@ -1493,7 +1497,7 @@
       </c>
     </row>
     <row spans="1:19" r="16">
-      <c r="A16" s="1" t="n">
+      <c s="1" r="A16" t="n">
         <v>14</v>
       </c>
       <c r="B16" t="s">
@@ -1552,7 +1556,7 @@
       </c>
     </row>
     <row spans="1:19" r="17">
-      <c r="A17" s="1" t="n">
+      <c s="1" r="A17" t="n">
         <v>15</v>
       </c>
       <c r="B17" t="s">
@@ -1611,7 +1615,7 @@
       </c>
     </row>
     <row spans="1:19" r="18">
-      <c r="A18" s="1" t="n">
+      <c s="1" r="A18" t="n">
         <v>16</v>
       </c>
       <c r="B18" t="s">
@@ -1670,7 +1674,7 @@
       </c>
     </row>
     <row spans="1:19" r="19">
-      <c r="A19" s="1" t="n">
+      <c s="1" r="A19" t="n">
         <v>17</v>
       </c>
       <c r="B19" t="s">
@@ -1748,63 +1752,63 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row spans="1:19" r="1">
-      <c r="B1" s="1" t="s">
+      <c s="1" r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c s="1" r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c s="1" r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c s="1" r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c s="1" r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c s="1" r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c s="1" r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c s="1" r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c s="1" r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c s="1" r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c s="1" r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c s="1" r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c s="1" r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c s="1" r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c s="1" r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c s="1" r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c s="1" r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c s="1" r="S1" t="s">
         <v>17</v>
       </c>
     </row>
     <row spans="1:19" r="2">
-      <c r="A2" s="1" t="n">
+      <c s="1" r="A2" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -1863,7 +1867,7 @@
       </c>
     </row>
     <row spans="1:19" r="3">
-      <c r="A3" s="1" t="n">
+      <c s="1" r="A3" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -1919,7 +1923,7 @@
       </c>
     </row>
     <row spans="1:19" r="4">
-      <c r="A4" s="1" t="n">
+      <c s="1" r="A4" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -1978,7 +1982,7 @@
       </c>
     </row>
     <row spans="1:19" r="5">
-      <c r="A5" s="1" t="n">
+      <c s="1" r="A5" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -2037,7 +2041,7 @@
       </c>
     </row>
     <row spans="1:19" r="6">
-      <c r="A6" s="1" t="n">
+      <c s="1" r="A6" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -2096,7 +2100,7 @@
       </c>
     </row>
     <row spans="1:19" r="7">
-      <c r="A7" s="1" t="n">
+      <c s="1" r="A7" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -2155,7 +2159,7 @@
       </c>
     </row>
     <row spans="1:19" r="8">
-      <c r="A8" s="1" t="n">
+      <c s="1" r="A8" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -2214,7 +2218,7 @@
       </c>
     </row>
     <row spans="1:19" r="9">
-      <c r="A9" s="1" t="n">
+      <c s="1" r="A9" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="s">
@@ -2273,7 +2277,7 @@
       </c>
     </row>
     <row spans="1:19" r="10">
-      <c r="A10" s="1" t="n">
+      <c s="1" r="A10" t="n">
         <v>8</v>
       </c>
       <c r="B10" t="s">
@@ -2332,7 +2336,7 @@
       </c>
     </row>
     <row spans="1:19" r="11">
-      <c r="A11" s="1" t="n">
+      <c s="1" r="A11" t="n">
         <v>9</v>
       </c>
       <c r="B11" t="s">
@@ -2391,7 +2395,7 @@
       </c>
     </row>
     <row spans="1:19" r="12">
-      <c r="A12" s="1" t="n">
+      <c s="1" r="A12" t="n">
         <v>10</v>
       </c>
       <c r="B12" t="s">
@@ -2450,7 +2454,7 @@
       </c>
     </row>
     <row spans="1:19" r="13">
-      <c r="A13" s="1" t="n">
+      <c s="1" r="A13" t="n">
         <v>11</v>
       </c>
       <c r="B13" t="s">
@@ -2509,7 +2513,7 @@
       </c>
     </row>
     <row spans="1:19" r="14">
-      <c r="A14" s="1" t="n">
+      <c s="1" r="A14" t="n">
         <v>12</v>
       </c>
       <c r="B14" t="s">
@@ -2568,7 +2572,7 @@
       </c>
     </row>
     <row spans="1:19" r="15">
-      <c r="A15" s="1" t="n">
+      <c s="1" r="A15" t="n">
         <v>13</v>
       </c>
       <c r="B15" t="s">
@@ -2627,7 +2631,7 @@
       </c>
     </row>
     <row spans="1:19" r="16">
-      <c r="A16" s="1" t="n">
+      <c s="1" r="A16" t="n">
         <v>14</v>
       </c>
       <c r="B16" t="s">
@@ -2686,7 +2690,7 @@
       </c>
     </row>
     <row spans="1:19" r="17">
-      <c r="A17" s="1" t="n">
+      <c s="1" r="A17" t="n">
         <v>15</v>
       </c>
       <c r="B17" t="s">
@@ -2745,7 +2749,7 @@
       </c>
     </row>
     <row spans="1:19" r="18">
-      <c r="A18" s="1" t="n">
+      <c s="1" r="A18" t="n">
         <v>16</v>
       </c>
       <c r="B18" t="s">
@@ -2804,7 +2808,7 @@
       </c>
     </row>
     <row spans="1:19" r="19">
-      <c r="A19" s="1" t="n">
+      <c s="1" r="A19" t="n">
         <v>17</v>
       </c>
       <c r="B19" t="s">
@@ -2863,7 +2867,7 @@
       </c>
     </row>
     <row spans="1:19" r="20">
-      <c r="A20" s="1" t="n">
+      <c s="1" r="A20" t="n">
         <v>18</v>
       </c>
       <c r="B20" t="s">
@@ -2922,7 +2926,7 @@
       </c>
     </row>
     <row spans="1:19" r="21">
-      <c r="A21" s="1" t="n">
+      <c s="1" r="A21" t="n">
         <v>19</v>
       </c>
       <c r="B21" t="s">
@@ -2981,7 +2985,7 @@
       </c>
     </row>
     <row spans="1:19" r="22">
-      <c r="A22" s="1" t="n">
+      <c s="1" r="A22" t="n">
         <v>20</v>
       </c>
       <c r="B22" t="s">
@@ -3040,7 +3044,7 @@
       </c>
     </row>
     <row spans="1:19" r="23">
-      <c r="A23" s="1" t="n">
+      <c s="1" r="A23" t="n">
         <v>21</v>
       </c>
       <c r="B23" t="s">
@@ -3099,7 +3103,7 @@
       </c>
     </row>
     <row spans="1:19" r="24">
-      <c r="A24" s="1" t="n">
+      <c s="1" r="A24" t="n">
         <v>22</v>
       </c>
       <c r="B24" t="s">
@@ -3158,7 +3162,7 @@
       </c>
     </row>
     <row spans="1:19" r="25">
-      <c r="A25" s="1" t="n">
+      <c s="1" r="A25" t="n">
         <v>23</v>
       </c>
       <c r="B25" t="s">
@@ -3217,7 +3221,7 @@
       </c>
     </row>
     <row spans="1:19" r="26">
-      <c r="A26" s="1" t="n">
+      <c s="1" r="A26" t="n">
         <v>24</v>
       </c>
       <c r="B26" t="s">
@@ -3276,7 +3280,7 @@
       </c>
     </row>
     <row spans="1:19" r="27">
-      <c r="A27" s="1" t="n">
+      <c s="1" r="A27" t="n">
         <v>25</v>
       </c>
       <c r="B27" t="s">
@@ -3335,7 +3339,7 @@
       </c>
     </row>
     <row spans="1:19" r="28">
-      <c r="A28" s="1" t="n">
+      <c s="1" r="A28" t="n">
         <v>26</v>
       </c>
       <c r="B28" t="s">
@@ -3394,7 +3398,7 @@
       </c>
     </row>
     <row spans="1:19" r="29">
-      <c r="A29" s="1" t="n">
+      <c s="1" r="A29" t="n">
         <v>27</v>
       </c>
       <c r="B29" t="s">
@@ -3453,7 +3457,7 @@
       </c>
     </row>
     <row spans="1:19" r="30">
-      <c r="A30" s="1" t="n">
+      <c s="1" r="A30" t="n">
         <v>28</v>
       </c>
       <c r="B30" t="s">
@@ -3512,7 +3516,7 @@
       </c>
     </row>
     <row spans="1:19" r="31">
-      <c r="A31" s="1" t="n">
+      <c s="1" r="A31" t="n">
         <v>29</v>
       </c>
       <c r="B31" t="s">
@@ -3571,7 +3575,7 @@
       </c>
     </row>
     <row spans="1:19" r="32">
-      <c r="A32" s="1" t="n">
+      <c s="1" r="A32" t="n">
         <v>30</v>
       </c>
       <c r="B32" t="s">
@@ -3630,7 +3634,7 @@
       </c>
     </row>
     <row spans="1:19" r="33">
-      <c r="A33" s="1" t="n">
+      <c s="1" r="A33" t="n">
         <v>31</v>
       </c>
       <c r="B33" t="s">
@@ -3708,78 +3712,78 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row spans="1:24" r="1">
-      <c r="B1" s="1" t="s">
+      <c s="1" r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c s="1" r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c s="1" r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c s="1" r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c s="1" r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c s="1" r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c s="1" r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c s="1" r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c s="1" r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c s="1" r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c s="1" r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c s="1" r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c s="1" r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c s="1" r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c s="1" r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c s="1" r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c s="1" r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c s="1" r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c s="1" r="T1" t="s">
         <v>58</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c s="1" r="U1" t="s">
         <v>59</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c s="1" r="V1" t="s">
         <v>60</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c s="1" r="W1" t="s">
         <v>61</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c s="1" r="X1" t="s">
         <v>62</v>
       </c>
     </row>
     <row spans="1:24" r="2">
-      <c r="A2" s="1" t="n">
+      <c s="1" r="A2" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -3853,7 +3857,7 @@
       </c>
     </row>
     <row spans="1:24" r="3">
-      <c r="A3" s="1" t="n">
+      <c s="1" r="A3" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -3927,7 +3931,7 @@
       </c>
     </row>
     <row spans="1:24" r="4">
-      <c r="A4" s="1" t="n">
+      <c s="1" r="A4" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -4001,7 +4005,7 @@
       </c>
     </row>
     <row spans="1:24" r="5">
-      <c r="A5" s="1" t="n">
+      <c s="1" r="A5" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -4075,7 +4079,7 @@
       </c>
     </row>
     <row spans="1:24" r="6">
-      <c r="A6" s="1" t="n">
+      <c s="1" r="A6" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -4149,7 +4153,7 @@
       </c>
     </row>
     <row spans="1:24" r="7">
-      <c r="A7" s="1" t="n">
+      <c s="1" r="A7" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -4223,7 +4227,7 @@
       </c>
     </row>
     <row spans="1:24" r="8">
-      <c r="A8" s="1" t="n">
+      <c s="1" r="A8" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -4297,7 +4301,7 @@
       </c>
     </row>
     <row spans="1:24" r="9">
-      <c r="A9" s="1" t="n">
+      <c s="1" r="A9" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="s">
@@ -4371,7 +4375,7 @@
       </c>
     </row>
     <row spans="1:24" r="10">
-      <c r="A10" s="1" t="n">
+      <c s="1" r="A10" t="n">
         <v>8</v>
       </c>
       <c r="B10" t="s">
@@ -4445,7 +4449,7 @@
       </c>
     </row>
     <row spans="1:24" r="11">
-      <c r="A11" s="1" t="n">
+      <c s="1" r="A11" t="n">
         <v>9</v>
       </c>
       <c r="B11" t="s">
@@ -4519,7 +4523,7 @@
       </c>
     </row>
     <row spans="1:24" r="12">
-      <c r="A12" s="1" t="n">
+      <c s="1" r="A12" t="n">
         <v>10</v>
       </c>
       <c r="B12" t="s">
@@ -4593,7 +4597,7 @@
       </c>
     </row>
     <row spans="1:24" r="13">
-      <c r="A13" s="1" t="n">
+      <c s="1" r="A13" t="n">
         <v>11</v>
       </c>
       <c r="B13" t="s">
@@ -4667,7 +4671,7 @@
       </c>
     </row>
     <row spans="1:24" r="14">
-      <c r="A14" s="1" t="n">
+      <c s="1" r="A14" t="n">
         <v>12</v>
       </c>
       <c r="B14" t="s">
@@ -4741,7 +4745,7 @@
       </c>
     </row>
     <row spans="1:24" r="15">
-      <c r="A15" s="1" t="n">
+      <c s="1" r="A15" t="n">
         <v>13</v>
       </c>
       <c r="B15" t="s">
@@ -4815,7 +4819,7 @@
       </c>
     </row>
     <row spans="1:24" r="16">
-      <c r="A16" s="1" t="n">
+      <c s="1" r="A16" t="n">
         <v>14</v>
       </c>
       <c r="B16" t="s">
@@ -4889,7 +4893,7 @@
       </c>
     </row>
     <row spans="1:24" r="17">
-      <c r="A17" s="1" t="n">
+      <c s="1" r="A17" t="n">
         <v>15</v>
       </c>
       <c r="B17" t="s">
@@ -4963,7 +4967,7 @@
       </c>
     </row>
     <row spans="1:24" r="18">
-      <c r="A18" s="1" t="n">
+      <c s="1" r="A18" t="n">
         <v>16</v>
       </c>
       <c r="B18" t="s">
@@ -5037,7 +5041,7 @@
       </c>
     </row>
     <row spans="1:24" r="19">
-      <c r="A19" s="1" t="n">
+      <c s="1" r="A19" t="n">
         <v>17</v>
       </c>
       <c r="B19" t="s">
@@ -5111,7 +5115,7 @@
       </c>
     </row>
     <row spans="1:24" r="20">
-      <c r="A20" s="1" t="n">
+      <c s="1" r="A20" t="n">
         <v>18</v>
       </c>
       <c r="B20" t="s">
@@ -5185,7 +5189,7 @@
       </c>
     </row>
     <row spans="1:24" r="21">
-      <c r="A21" s="1" t="n">
+      <c s="1" r="A21" t="n">
         <v>19</v>
       </c>
       <c r="B21" t="s">
@@ -5259,7 +5263,7 @@
       </c>
     </row>
     <row spans="1:24" r="22">
-      <c r="A22" s="1" t="n">
+      <c s="1" r="A22" t="n">
         <v>20</v>
       </c>
       <c r="B22" t="s">
@@ -5333,7 +5337,7 @@
       </c>
     </row>
     <row spans="1:24" r="23">
-      <c r="A23" s="1" t="n">
+      <c s="1" r="A23" t="n">
         <v>21</v>
       </c>
       <c r="B23" t="s">
@@ -5407,7 +5411,7 @@
       </c>
     </row>
     <row spans="1:24" r="24">
-      <c r="A24" s="1" t="n">
+      <c s="1" r="A24" t="n">
         <v>22</v>
       </c>
       <c r="B24" t="s">
@@ -5481,7 +5485,7 @@
       </c>
     </row>
     <row spans="1:24" r="25">
-      <c r="A25" s="1" t="n">
+      <c s="1" r="A25" t="n">
         <v>23</v>
       </c>
       <c r="B25" t="s">
@@ -5555,7 +5559,7 @@
       </c>
     </row>
     <row spans="1:24" r="26">
-      <c r="A26" s="1" t="n">
+      <c s="1" r="A26" t="n">
         <v>24</v>
       </c>
       <c r="B26" t="s">
@@ -5629,7 +5633,7 @@
       </c>
     </row>
     <row spans="1:24" r="27">
-      <c r="A27" s="1" t="n">
+      <c s="1" r="A27" t="n">
         <v>25</v>
       </c>
       <c r="B27" t="s">
@@ -5703,7 +5707,7 @@
       </c>
     </row>
     <row spans="1:24" r="28">
-      <c r="A28" s="1" t="n">
+      <c s="1" r="A28" t="n">
         <v>26</v>
       </c>
       <c r="B28" t="s">
@@ -5777,7 +5781,7 @@
       </c>
     </row>
     <row spans="1:24" r="29">
-      <c r="A29" s="1" t="n">
+      <c s="1" r="A29" t="n">
         <v>27</v>
       </c>
       <c r="B29" t="s">
@@ -5851,7 +5855,7 @@
       </c>
     </row>
     <row spans="1:24" r="30">
-      <c r="A30" s="1" t="n">
+      <c s="1" r="A30" t="n">
         <v>28</v>
       </c>
       <c r="B30" t="s">
@@ -5925,7 +5929,7 @@
       </c>
     </row>
     <row spans="1:24" r="31">
-      <c r="A31" s="1" t="n">
+      <c s="1" r="A31" t="n">
         <v>29</v>
       </c>
       <c r="B31" t="s">
@@ -5999,7 +6003,7 @@
       </c>
     </row>
     <row spans="1:24" r="32">
-      <c r="A32" s="1" t="n">
+      <c s="1" r="A32" t="n">
         <v>30</v>
       </c>
       <c r="B32" t="s">
@@ -6073,7 +6077,7 @@
       </c>
     </row>
     <row spans="1:24" r="33">
-      <c r="A33" s="1" t="n">
+      <c s="1" r="A33" t="n">
         <v>31</v>
       </c>
       <c r="B33" t="s">
@@ -6147,7 +6151,7 @@
       </c>
     </row>
     <row spans="1:24" r="34">
-      <c r="A34" s="1" t="n">
+      <c s="1" r="A34" t="n">
         <v>32</v>
       </c>
       <c r="B34" t="s">
@@ -6221,7 +6225,7 @@
       </c>
     </row>
     <row spans="1:24" r="35">
-      <c r="A35" s="1" t="n">
+      <c s="1" r="A35" t="n">
         <v>33</v>
       </c>
       <c r="B35" t="s">
@@ -6295,7 +6299,7 @@
       </c>
     </row>
     <row spans="1:24" r="36">
-      <c r="A36" s="1" t="n">
+      <c s="1" r="A36" t="n">
         <v>34</v>
       </c>
       <c r="B36" t="s">
@@ -6369,7 +6373,7 @@
       </c>
     </row>
     <row spans="1:24" r="37">
-      <c r="A37" s="1" t="n">
+      <c s="1" r="A37" t="n">
         <v>35</v>
       </c>
       <c r="B37" t="s">
@@ -6443,7 +6447,7 @@
       </c>
     </row>
     <row spans="1:24" r="38">
-      <c r="A38" s="1" t="n">
+      <c s="1" r="A38" t="n">
         <v>36</v>
       </c>
       <c r="B38" t="s">
@@ -6517,7 +6521,7 @@
       </c>
     </row>
     <row spans="1:24" r="39">
-      <c r="A39" s="1" t="n">
+      <c s="1" r="A39" t="n">
         <v>37</v>
       </c>
       <c r="B39" t="s">
@@ -6591,7 +6595,7 @@
       </c>
     </row>
     <row spans="1:24" r="40">
-      <c r="A40" s="1" t="n">
+      <c s="1" r="A40" t="n">
         <v>38</v>
       </c>
       <c r="B40" t="s">
@@ -6665,7 +6669,7 @@
       </c>
     </row>
     <row spans="1:24" r="41">
-      <c r="A41" s="1" t="n">
+      <c s="1" r="A41" t="n">
         <v>39</v>
       </c>
       <c r="B41" t="s">
@@ -6739,7 +6743,7 @@
       </c>
     </row>
     <row spans="1:24" r="42">
-      <c r="A42" s="1" t="n">
+      <c s="1" r="A42" t="n">
         <v>40</v>
       </c>
       <c r="B42" t="s">
@@ -6813,7 +6817,7 @@
       </c>
     </row>
     <row spans="1:24" r="43">
-      <c r="A43" s="1" t="n">
+      <c s="1" r="A43" t="n">
         <v>41</v>
       </c>
       <c r="B43" t="s">
@@ -6887,7 +6891,7 @@
       </c>
     </row>
     <row spans="1:24" r="44">
-      <c r="A44" s="1" t="n">
+      <c s="1" r="A44" t="n">
         <v>42</v>
       </c>
       <c r="B44" t="s">
@@ -6961,7 +6965,7 @@
       </c>
     </row>
     <row spans="1:24" r="45">
-      <c r="A45" s="1" t="n">
+      <c s="1" r="A45" t="n">
         <v>43</v>
       </c>
       <c r="B45" t="s">
@@ -7035,7 +7039,7 @@
       </c>
     </row>
     <row spans="1:24" r="46">
-      <c r="A46" s="1" t="n">
+      <c s="1" r="A46" t="n">
         <v>44</v>
       </c>
       <c r="B46" t="s">
@@ -7109,7 +7113,7 @@
       </c>
     </row>
     <row spans="1:24" r="47">
-      <c r="A47" s="1" t="n">
+      <c s="1" r="A47" t="n">
         <v>45</v>
       </c>
       <c r="B47" t="s">
@@ -7183,11 +7187,3579 @@
       </c>
     </row>
     <row spans="1:24" r="48">
-      <c r="A48" s="1" t="n">
+      <c s="1" r="A48" t="n">
         <v>46</v>
       </c>
       <c r="B48" t="s">
         <v>20</v>
+      </c>
+      <c r="C48" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" t="n">
+        <v>16.685</v>
+      </c>
+      <c r="E48" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" t="n">
+        <v>17.77</v>
+      </c>
+      <c r="G48" t="n">
+        <v>15.876</v>
+      </c>
+      <c r="H48" t="n">
+        <v>17.472</v>
+      </c>
+      <c r="I48" t="s">
+        <v>25</v>
+      </c>
+      <c r="J48" t="s">
+        <v>63</v>
+      </c>
+      <c r="K48" t="n">
+        <v>17.77</v>
+      </c>
+      <c r="L48" t="n">
+        <v>15.876</v>
+      </c>
+      <c r="M48" t="n">
+        <v>17.472</v>
+      </c>
+      <c r="N48" t="s">
+        <v>25</v>
+      </c>
+      <c r="O48" t="s">
+        <v>22</v>
+      </c>
+      <c r="P48" t="n">
+        <v>17.369</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>14.275</v>
+      </c>
+      <c r="R48" t="n">
+        <v>17.185</v>
+      </c>
+      <c r="S48" t="s">
+        <v>25</v>
+      </c>
+      <c r="T48" t="s">
+        <v>23</v>
+      </c>
+      <c r="U48" t="n">
+        <v>17.369</v>
+      </c>
+      <c r="V48" t="n">
+        <v>14.275</v>
+      </c>
+      <c r="W48" t="n">
+        <v>17.185</v>
+      </c>
+      <c r="X48" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:X48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row spans="1:24" r="1">
+      <c s="1" r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c s="1" r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c s="1" r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c s="1" r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c s="1" r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c s="1" r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c s="1" r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c s="1" r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c s="1" r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c s="1" r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c s="1" r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c s="1" r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c s="1" r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c s="1" r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c s="1" r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c s="1" r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c s="1" r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c s="1" r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c s="1" r="T1" t="s">
+        <v>58</v>
+      </c>
+      <c s="1" r="U1" t="s">
+        <v>59</v>
+      </c>
+      <c s="1" r="V1" t="s">
+        <v>60</v>
+      </c>
+      <c s="1" r="W1" t="s">
+        <v>61</v>
+      </c>
+      <c s="1" r="X1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row spans="1:24" r="2">
+      <c s="1" r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="n">
+        <v>170.515</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="n">
+        <v>175.284</v>
+      </c>
+      <c r="G2" t="n">
+        <v>163.349</v>
+      </c>
+      <c r="H2" t="n">
+        <v>170.21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K2" t="n">
+        <v>175.284</v>
+      </c>
+      <c r="L2" t="n">
+        <v>163.349</v>
+      </c>
+      <c r="M2" t="n">
+        <v>170.21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" t="n">
+        <v>181.915</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>162.195</v>
+      </c>
+      <c r="R2" t="n">
+        <v>174.346</v>
+      </c>
+      <c r="S2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T2" t="s">
+        <v>23</v>
+      </c>
+      <c r="U2" t="n">
+        <v>179.171</v>
+      </c>
+      <c r="V2" t="n">
+        <v>135.543</v>
+      </c>
+      <c r="W2" t="n">
+        <v>165.938</v>
+      </c>
+      <c r="X2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="3">
+      <c s="1" r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="n">
+        <v>54.03</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="n">
+        <v>56.455</v>
+      </c>
+      <c r="G3" t="n">
+        <v>52.545</v>
+      </c>
+      <c r="H3" t="n">
+        <v>53.21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" t="n">
+        <v>56.455</v>
+      </c>
+      <c r="L3" t="n">
+        <v>52.545</v>
+      </c>
+      <c r="M3" t="n">
+        <v>53.21</v>
+      </c>
+      <c r="N3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" t="n">
+        <v>60.77</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>49.884</v>
+      </c>
+      <c r="R3" t="n">
+        <v>57.884</v>
+      </c>
+      <c r="S3" t="s">
+        <v>25</v>
+      </c>
+      <c r="T3" t="s">
+        <v>23</v>
+      </c>
+      <c r="U3" t="n">
+        <v>68.06999999999999</v>
+      </c>
+      <c r="V3" t="n">
+        <v>44.026</v>
+      </c>
+      <c r="W3" t="n">
+        <v>62.81</v>
+      </c>
+      <c r="X3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="4">
+      <c s="1" r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2.09</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3.472</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="H4" t="n">
+        <v>3.472</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" t="n">
+        <v>3.472</v>
+      </c>
+      <c r="L4" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="M4" t="n">
+        <v>3.472</v>
+      </c>
+      <c r="N4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" t="n">
+        <v>3.535</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>1.862</v>
+      </c>
+      <c r="R4" t="n">
+        <v>2.548</v>
+      </c>
+      <c r="S4" t="s">
+        <v>21</v>
+      </c>
+      <c r="T4" t="s">
+        <v>23</v>
+      </c>
+      <c r="U4" t="n">
+        <v>3.535</v>
+      </c>
+      <c r="V4" t="n">
+        <v>1.862</v>
+      </c>
+      <c r="W4" t="n">
+        <v>2.548</v>
+      </c>
+      <c r="X4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row spans="1:24" r="5">
+      <c s="1" r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="n">
+        <v>11.515</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="n">
+        <v>12.637</v>
+      </c>
+      <c r="G5" t="n">
+        <v>11.083</v>
+      </c>
+      <c r="H5" t="n">
+        <v>12.323</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" t="n">
+        <v>12.637</v>
+      </c>
+      <c r="L5" t="n">
+        <v>11.083</v>
+      </c>
+      <c r="M5" t="n">
+        <v>12.323</v>
+      </c>
+      <c r="N5" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P5" t="n">
+        <v>12.954</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>10.403</v>
+      </c>
+      <c r="R5" t="n">
+        <v>12.444</v>
+      </c>
+      <c r="S5" t="s">
+        <v>25</v>
+      </c>
+      <c r="T5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U5" t="n">
+        <v>13.894</v>
+      </c>
+      <c r="V5" t="n">
+        <v>10.451</v>
+      </c>
+      <c r="W5" t="n">
+        <v>13.114</v>
+      </c>
+      <c r="X5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="6">
+      <c s="1" r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" t="n">
+        <v>59.97</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="n">
+        <v>64.428</v>
+      </c>
+      <c r="G6" t="n">
+        <v>51.815</v>
+      </c>
+      <c r="H6" t="n">
+        <v>54.71</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J6" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" t="n">
+        <v>64.428</v>
+      </c>
+      <c r="L6" t="n">
+        <v>51.815</v>
+      </c>
+      <c r="M6" t="n">
+        <v>54.71</v>
+      </c>
+      <c r="N6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" t="n">
+        <v>66.273</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>39.596</v>
+      </c>
+      <c r="R6" t="n">
+        <v>58.864</v>
+      </c>
+      <c r="S6" t="s">
+        <v>25</v>
+      </c>
+      <c r="T6" t="s">
+        <v>23</v>
+      </c>
+      <c r="U6" t="n">
+        <v>66.273</v>
+      </c>
+      <c r="V6" t="n">
+        <v>39.596</v>
+      </c>
+      <c r="W6" t="n">
+        <v>58.864</v>
+      </c>
+      <c r="X6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="7">
+      <c s="1" r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="n">
+        <v>63.81</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="n">
+        <v>65.29300000000001</v>
+      </c>
+      <c r="G7" t="n">
+        <v>58.844</v>
+      </c>
+      <c r="H7" t="n">
+        <v>64.36199999999999</v>
+      </c>
+      <c r="I7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" t="n">
+        <v>65.29300000000001</v>
+      </c>
+      <c r="L7" t="n">
+        <v>58.844</v>
+      </c>
+      <c r="M7" t="n">
+        <v>64.36199999999999</v>
+      </c>
+      <c r="N7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" t="s">
+        <v>22</v>
+      </c>
+      <c r="P7" t="n">
+        <v>66.874</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>56.188</v>
+      </c>
+      <c r="R7" t="n">
+        <v>63.262</v>
+      </c>
+      <c r="S7" t="s">
+        <v>21</v>
+      </c>
+      <c r="T7" t="s">
+        <v>23</v>
+      </c>
+      <c r="U7" t="n">
+        <v>66.88800000000001</v>
+      </c>
+      <c r="V7" t="n">
+        <v>49.234</v>
+      </c>
+      <c r="W7" t="n">
+        <v>62.868</v>
+      </c>
+      <c r="X7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="8">
+      <c s="1" r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="n">
+        <v>185.585</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="n">
+        <v>189.687</v>
+      </c>
+      <c r="G8" t="n">
+        <v>177.879</v>
+      </c>
+      <c r="H8" t="n">
+        <v>184.818</v>
+      </c>
+      <c r="I8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" t="n">
+        <v>189.687</v>
+      </c>
+      <c r="L8" t="n">
+        <v>177.879</v>
+      </c>
+      <c r="M8" t="n">
+        <v>184.818</v>
+      </c>
+      <c r="N8" t="s">
+        <v>21</v>
+      </c>
+      <c r="O8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P8" t="n">
+        <v>194.62</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>176.431</v>
+      </c>
+      <c r="R8" t="n">
+        <v>184.818</v>
+      </c>
+      <c r="S8" t="s">
+        <v>21</v>
+      </c>
+      <c r="T8" t="s">
+        <v>23</v>
+      </c>
+      <c r="U8" t="n">
+        <v>193.741</v>
+      </c>
+      <c r="V8" t="n">
+        <v>152.951</v>
+      </c>
+      <c r="W8" t="n">
+        <v>183.247</v>
+      </c>
+      <c r="X8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="9">
+      <c s="1" r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="n">
+        <v>241.025</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="n">
+        <v>247.732</v>
+      </c>
+      <c r="G9" t="n">
+        <v>225.157</v>
+      </c>
+      <c r="H9" t="n">
+        <v>239.496</v>
+      </c>
+      <c r="I9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" t="n">
+        <v>247.732</v>
+      </c>
+      <c r="L9" t="n">
+        <v>225.157</v>
+      </c>
+      <c r="M9" t="n">
+        <v>239.496</v>
+      </c>
+      <c r="N9" t="s">
+        <v>21</v>
+      </c>
+      <c r="O9" t="s">
+        <v>22</v>
+      </c>
+      <c r="P9" t="n">
+        <v>264.486</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>221.705</v>
+      </c>
+      <c r="R9" t="n">
+        <v>247.639</v>
+      </c>
+      <c r="S9" t="s">
+        <v>21</v>
+      </c>
+      <c r="T9" t="s">
+        <v>23</v>
+      </c>
+      <c r="U9" t="n">
+        <v>256.907</v>
+      </c>
+      <c r="V9" t="n">
+        <v>188.27</v>
+      </c>
+      <c r="W9" t="n">
+        <v>236.122</v>
+      </c>
+      <c r="X9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="10">
+      <c s="1" r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="n">
+        <v>47.69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" t="n">
+        <v>48.809</v>
+      </c>
+      <c r="G10" t="n">
+        <v>46.396</v>
+      </c>
+      <c r="H10" t="n">
+        <v>48.176</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>63</v>
+      </c>
+      <c r="K10" t="n">
+        <v>48.809</v>
+      </c>
+      <c r="L10" t="n">
+        <v>46.396</v>
+      </c>
+      <c r="M10" t="n">
+        <v>48.176</v>
+      </c>
+      <c r="N10" t="s">
+        <v>25</v>
+      </c>
+      <c r="O10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P10" t="n">
+        <v>49.375</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>44.213</v>
+      </c>
+      <c r="R10" t="n">
+        <v>47.095</v>
+      </c>
+      <c r="S10" t="s">
+        <v>21</v>
+      </c>
+      <c r="T10" t="s">
+        <v>23</v>
+      </c>
+      <c r="U10" t="n">
+        <v>53.625</v>
+      </c>
+      <c r="V10" t="n">
+        <v>44.191</v>
+      </c>
+      <c r="W10" t="n">
+        <v>49.654</v>
+      </c>
+      <c r="X10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row spans="1:24" r="11">
+      <c s="1" r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="n">
+        <v>179.44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" t="n">
+        <v>182.203</v>
+      </c>
+      <c r="G11" t="n">
+        <v>171.558</v>
+      </c>
+      <c r="H11" t="n">
+        <v>178.047</v>
+      </c>
+      <c r="I11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" t="s">
+        <v>63</v>
+      </c>
+      <c r="K11" t="n">
+        <v>182.203</v>
+      </c>
+      <c r="L11" t="n">
+        <v>171.558</v>
+      </c>
+      <c r="M11" t="n">
+        <v>178.047</v>
+      </c>
+      <c r="N11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" t="s">
+        <v>22</v>
+      </c>
+      <c r="P11" t="n">
+        <v>186.988</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>168.287</v>
+      </c>
+      <c r="R11" t="n">
+        <v>178.041</v>
+      </c>
+      <c r="S11" t="s">
+        <v>21</v>
+      </c>
+      <c r="T11" t="s">
+        <v>23</v>
+      </c>
+      <c r="U11" t="n">
+        <v>193.408</v>
+      </c>
+      <c r="V11" t="n">
+        <v>133.448</v>
+      </c>
+      <c r="W11" t="n">
+        <v>174.64</v>
+      </c>
+      <c r="X11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="12">
+      <c s="1" r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="n">
+        <v>6.135</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="n">
+        <v>6.548</v>
+      </c>
+      <c r="G12" t="n">
+        <v>5.578</v>
+      </c>
+      <c r="H12" t="n">
+        <v>6.195</v>
+      </c>
+      <c r="I12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K12" t="n">
+        <v>6.548</v>
+      </c>
+      <c r="L12" t="n">
+        <v>5.578</v>
+      </c>
+      <c r="M12" t="n">
+        <v>6.195</v>
+      </c>
+      <c r="N12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P12" t="n">
+        <v>6.802</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>5.843</v>
+      </c>
+      <c r="R12" t="n">
+        <v>6.351</v>
+      </c>
+      <c r="S12" t="s">
+        <v>21</v>
+      </c>
+      <c r="T12" t="s">
+        <v>23</v>
+      </c>
+      <c r="U12" t="n">
+        <v>10.549</v>
+      </c>
+      <c r="V12" t="n">
+        <v>4.564</v>
+      </c>
+      <c r="W12" t="n">
+        <v>7.334</v>
+      </c>
+      <c r="X12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row spans="1:24" r="13">
+      <c s="1" r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" t="n">
+        <v>16.365</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" t="n">
+        <v>18.708</v>
+      </c>
+      <c r="G13" t="n">
+        <v>16.372</v>
+      </c>
+      <c r="H13" t="n">
+        <v>16.574</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" t="s">
+        <v>63</v>
+      </c>
+      <c r="K13" t="n">
+        <v>18.708</v>
+      </c>
+      <c r="L13" t="n">
+        <v>16.372</v>
+      </c>
+      <c r="M13" t="n">
+        <v>16.574</v>
+      </c>
+      <c r="N13" t="s">
+        <v>36</v>
+      </c>
+      <c r="O13" t="s">
+        <v>22</v>
+      </c>
+      <c r="P13" t="n">
+        <v>17.739</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>15.054</v>
+      </c>
+      <c r="R13" t="n">
+        <v>17.554</v>
+      </c>
+      <c r="S13" t="s">
+        <v>25</v>
+      </c>
+      <c r="T13" t="s">
+        <v>23</v>
+      </c>
+      <c r="U13" t="n">
+        <v>23.088</v>
+      </c>
+      <c r="V13" t="n">
+        <v>15.802</v>
+      </c>
+      <c r="W13" t="n">
+        <v>18.098</v>
+      </c>
+      <c r="X13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row spans="1:24" r="14">
+      <c s="1" r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1026.085</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1053.58</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1000.651</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1032.058</v>
+      </c>
+      <c r="I14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1053.58</v>
+      </c>
+      <c r="L14" t="n">
+        <v>1000.651</v>
+      </c>
+      <c r="M14" t="n">
+        <v>1032.058</v>
+      </c>
+      <c r="N14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O14" t="s">
+        <v>22</v>
+      </c>
+      <c r="P14" t="n">
+        <v>1108.602</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>920.89</v>
+      </c>
+      <c r="R14" t="n">
+        <v>1038.812</v>
+      </c>
+      <c r="S14" t="s">
+        <v>21</v>
+      </c>
+      <c r="T14" t="s">
+        <v>23</v>
+      </c>
+      <c r="U14" t="n">
+        <v>1085.746</v>
+      </c>
+      <c r="V14" t="n">
+        <v>716.287</v>
+      </c>
+      <c r="W14" t="n">
+        <v>991.145</v>
+      </c>
+      <c r="X14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="15">
+      <c s="1" r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="n">
+        <v>8.359999999999999</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" t="n">
+        <v>9.881</v>
+      </c>
+      <c r="G15" t="n">
+        <v>8.525</v>
+      </c>
+      <c r="H15" t="n">
+        <v>9.401999999999999</v>
+      </c>
+      <c r="I15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" t="s">
+        <v>63</v>
+      </c>
+      <c r="K15" t="n">
+        <v>9.881</v>
+      </c>
+      <c r="L15" t="n">
+        <v>8.525</v>
+      </c>
+      <c r="M15" t="n">
+        <v>9.401999999999999</v>
+      </c>
+      <c r="N15" t="s">
+        <v>21</v>
+      </c>
+      <c r="O15" t="s">
+        <v>22</v>
+      </c>
+      <c r="P15" t="n">
+        <v>10.002</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>8.378</v>
+      </c>
+      <c r="R15" t="n">
+        <v>9.007</v>
+      </c>
+      <c r="S15" t="s">
+        <v>21</v>
+      </c>
+      <c r="T15" t="s">
+        <v>23</v>
+      </c>
+      <c r="U15" t="n">
+        <v>12.98</v>
+      </c>
+      <c r="V15" t="n">
+        <v>6.372</v>
+      </c>
+      <c r="W15" t="n">
+        <v>9.214</v>
+      </c>
+      <c r="X15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row spans="1:24" r="16">
+      <c s="1" r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" t="n">
+        <v>61.18</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" t="n">
+        <v>61.705</v>
+      </c>
+      <c r="G16" t="n">
+        <v>56.253</v>
+      </c>
+      <c r="H16" t="n">
+        <v>61.599</v>
+      </c>
+      <c r="I16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" t="s">
+        <v>63</v>
+      </c>
+      <c r="K16" t="n">
+        <v>61.705</v>
+      </c>
+      <c r="L16" t="n">
+        <v>56.253</v>
+      </c>
+      <c r="M16" t="n">
+        <v>61.599</v>
+      </c>
+      <c r="N16" t="s">
+        <v>25</v>
+      </c>
+      <c r="O16" t="s">
+        <v>22</v>
+      </c>
+      <c r="P16" t="n">
+        <v>62.375</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>57.193</v>
+      </c>
+      <c r="R16" t="n">
+        <v>60.043</v>
+      </c>
+      <c r="S16" t="s">
+        <v>21</v>
+      </c>
+      <c r="T16" t="s">
+        <v>23</v>
+      </c>
+      <c r="U16" t="n">
+        <v>62.194</v>
+      </c>
+      <c r="V16" t="n">
+        <v>39.953</v>
+      </c>
+      <c r="W16" t="n">
+        <v>53.214</v>
+      </c>
+      <c r="X16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row spans="1:24" r="17">
+      <c s="1" r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" t="n">
+        <v>5.48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" t="n">
+        <v>5.593</v>
+      </c>
+      <c r="G17" t="n">
+        <v>4.804</v>
+      </c>
+      <c r="H17" t="n">
+        <v>5.422</v>
+      </c>
+      <c r="I17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" t="s">
+        <v>63</v>
+      </c>
+      <c r="K17" t="n">
+        <v>5.593</v>
+      </c>
+      <c r="L17" t="n">
+        <v>4.804</v>
+      </c>
+      <c r="M17" t="n">
+        <v>5.422</v>
+      </c>
+      <c r="N17" t="s">
+        <v>25</v>
+      </c>
+      <c r="O17" t="s">
+        <v>22</v>
+      </c>
+      <c r="P17" t="n">
+        <v>5.98</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>4.927</v>
+      </c>
+      <c r="R17" t="n">
+        <v>5.827</v>
+      </c>
+      <c r="S17" t="s">
+        <v>25</v>
+      </c>
+      <c r="T17" t="s">
+        <v>23</v>
+      </c>
+      <c r="U17" t="n">
+        <v>5.776</v>
+      </c>
+      <c r="V17" t="n">
+        <v>4.614</v>
+      </c>
+      <c r="W17" t="n">
+        <v>5.655</v>
+      </c>
+      <c r="X17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="18">
+      <c s="1" r="A18" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" t="n">
+        <v>42.52</v>
+      </c>
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" t="n">
+        <v>44.646</v>
+      </c>
+      <c r="G18" t="n">
+        <v>39.955</v>
+      </c>
+      <c r="H18" t="n">
+        <v>40.014</v>
+      </c>
+      <c r="I18" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" t="s">
+        <v>63</v>
+      </c>
+      <c r="K18" t="n">
+        <v>44.646</v>
+      </c>
+      <c r="L18" t="n">
+        <v>39.955</v>
+      </c>
+      <c r="M18" t="n">
+        <v>40.014</v>
+      </c>
+      <c r="N18" t="s">
+        <v>36</v>
+      </c>
+      <c r="O18" t="s">
+        <v>22</v>
+      </c>
+      <c r="P18" t="n">
+        <v>43.401</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>27.035</v>
+      </c>
+      <c r="R18" t="n">
+        <v>41.325</v>
+      </c>
+      <c r="S18" t="s">
+        <v>25</v>
+      </c>
+      <c r="T18" t="s">
+        <v>23</v>
+      </c>
+      <c r="U18" t="n">
+        <v>43.401</v>
+      </c>
+      <c r="V18" t="n">
+        <v>27.035</v>
+      </c>
+      <c r="W18" t="n">
+        <v>41.325</v>
+      </c>
+      <c r="X18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="19">
+      <c s="1" r="A19" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="n">
+        <v>40.34</v>
+      </c>
+      <c r="E19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" t="n">
+        <v>41.352</v>
+      </c>
+      <c r="G19" t="n">
+        <v>38.18</v>
+      </c>
+      <c r="H19" t="n">
+        <v>40.631</v>
+      </c>
+      <c r="I19" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" t="s">
+        <v>63</v>
+      </c>
+      <c r="K19" t="n">
+        <v>41.352</v>
+      </c>
+      <c r="L19" t="n">
+        <v>38.18</v>
+      </c>
+      <c r="M19" t="n">
+        <v>40.631</v>
+      </c>
+      <c r="N19" t="s">
+        <v>25</v>
+      </c>
+      <c r="O19" t="s">
+        <v>22</v>
+      </c>
+      <c r="P19" t="n">
+        <v>42.121</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>37.754</v>
+      </c>
+      <c r="R19" t="n">
+        <v>41.177</v>
+      </c>
+      <c r="S19" t="s">
+        <v>25</v>
+      </c>
+      <c r="T19" t="s">
+        <v>23</v>
+      </c>
+      <c r="U19" t="n">
+        <v>44.481</v>
+      </c>
+      <c r="V19" t="n">
+        <v>36.225</v>
+      </c>
+      <c r="W19" t="n">
+        <v>41.853</v>
+      </c>
+      <c r="X19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="20">
+      <c s="1" r="A20" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" t="n">
+        <v>4.964</v>
+      </c>
+      <c r="G20" t="n">
+        <v>4.209</v>
+      </c>
+      <c r="H20" t="n">
+        <v>4.56</v>
+      </c>
+      <c r="I20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" t="s">
+        <v>63</v>
+      </c>
+      <c r="K20" t="n">
+        <v>4.964</v>
+      </c>
+      <c r="L20" t="n">
+        <v>4.209</v>
+      </c>
+      <c r="M20" t="n">
+        <v>4.56</v>
+      </c>
+      <c r="N20" t="s">
+        <v>21</v>
+      </c>
+      <c r="O20" t="s">
+        <v>22</v>
+      </c>
+      <c r="P20" t="n">
+        <v>7.408</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>4.039</v>
+      </c>
+      <c r="R20" t="n">
+        <v>6.326</v>
+      </c>
+      <c r="S20" t="s">
+        <v>25</v>
+      </c>
+      <c r="T20" t="s">
+        <v>23</v>
+      </c>
+      <c r="U20" t="n">
+        <v>7.408</v>
+      </c>
+      <c r="V20" t="n">
+        <v>4.039</v>
+      </c>
+      <c r="W20" t="n">
+        <v>6.326</v>
+      </c>
+      <c r="X20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="21">
+      <c s="1" r="A21" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" t="n">
+        <v>6.23</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" t="n">
+        <v>7.288</v>
+      </c>
+      <c r="G21" t="n">
+        <v>5.573</v>
+      </c>
+      <c r="H21" t="n">
+        <v>7.059</v>
+      </c>
+      <c r="I21" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21" t="s">
+        <v>63</v>
+      </c>
+      <c r="K21" t="n">
+        <v>7.288</v>
+      </c>
+      <c r="L21" t="n">
+        <v>5.573</v>
+      </c>
+      <c r="M21" t="n">
+        <v>7.059</v>
+      </c>
+      <c r="N21" t="s">
+        <v>25</v>
+      </c>
+      <c r="O21" t="s">
+        <v>22</v>
+      </c>
+      <c r="P21" t="n">
+        <v>7.116</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>4.63</v>
+      </c>
+      <c r="R21" t="n">
+        <v>7.032</v>
+      </c>
+      <c r="S21" t="s">
+        <v>25</v>
+      </c>
+      <c r="T21" t="s">
+        <v>23</v>
+      </c>
+      <c r="U21" t="n">
+        <v>7.116</v>
+      </c>
+      <c r="V21" t="n">
+        <v>4.63</v>
+      </c>
+      <c r="W21" t="n">
+        <v>7.032</v>
+      </c>
+      <c r="X21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="22">
+      <c s="1" r="A22" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" t="n">
+        <v>32.25</v>
+      </c>
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" t="n">
+        <v>32.365</v>
+      </c>
+      <c r="G22" t="n">
+        <v>29.433</v>
+      </c>
+      <c r="H22" t="n">
+        <v>31.721</v>
+      </c>
+      <c r="I22" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" t="s">
+        <v>63</v>
+      </c>
+      <c r="K22" t="n">
+        <v>32.365</v>
+      </c>
+      <c r="L22" t="n">
+        <v>29.433</v>
+      </c>
+      <c r="M22" t="n">
+        <v>31.721</v>
+      </c>
+      <c r="N22" t="s">
+        <v>25</v>
+      </c>
+      <c r="O22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P22" t="n">
+        <v>34.547</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>26.866</v>
+      </c>
+      <c r="R22" t="n">
+        <v>32.419</v>
+      </c>
+      <c r="S22" t="s">
+        <v>25</v>
+      </c>
+      <c r="T22" t="s">
+        <v>23</v>
+      </c>
+      <c r="U22" t="n">
+        <v>42.755</v>
+      </c>
+      <c r="V22" t="n">
+        <v>28.962</v>
+      </c>
+      <c r="W22" t="n">
+        <v>37.565</v>
+      </c>
+      <c r="X22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row spans="1:24" r="23">
+      <c s="1" r="A23" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" t="n">
+        <v>20.345</v>
+      </c>
+      <c r="E23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" t="n">
+        <v>20.345</v>
+      </c>
+      <c r="G23" t="n">
+        <v>19.608</v>
+      </c>
+      <c r="H23" t="n">
+        <v>20.083</v>
+      </c>
+      <c r="I23" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" t="s">
+        <v>63</v>
+      </c>
+      <c r="K23" t="n">
+        <v>20.345</v>
+      </c>
+      <c r="L23" t="n">
+        <v>19.608</v>
+      </c>
+      <c r="M23" t="n">
+        <v>20.083</v>
+      </c>
+      <c r="N23" t="s">
+        <v>21</v>
+      </c>
+      <c r="O23" t="s">
+        <v>22</v>
+      </c>
+      <c r="P23" t="n">
+        <v>21.526</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>18.962</v>
+      </c>
+      <c r="R23" t="n">
+        <v>20.617</v>
+      </c>
+      <c r="S23" t="s">
+        <v>21</v>
+      </c>
+      <c r="T23" t="s">
+        <v>23</v>
+      </c>
+      <c r="U23" t="n">
+        <v>20.469</v>
+      </c>
+      <c r="V23" t="n">
+        <v>13.835</v>
+      </c>
+      <c r="W23" t="n">
+        <v>18.827</v>
+      </c>
+      <c r="X23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="24">
+      <c s="1" r="A24" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" t="n">
+        <v>82.68000000000001</v>
+      </c>
+      <c r="E24" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" t="n">
+        <v>84.145</v>
+      </c>
+      <c r="G24" t="n">
+        <v>80.497</v>
+      </c>
+      <c r="H24" t="n">
+        <v>82.033</v>
+      </c>
+      <c r="I24" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" t="s">
+        <v>63</v>
+      </c>
+      <c r="K24" t="n">
+        <v>84.145</v>
+      </c>
+      <c r="L24" t="n">
+        <v>80.497</v>
+      </c>
+      <c r="M24" t="n">
+        <v>82.033</v>
+      </c>
+      <c r="N24" t="s">
+        <v>21</v>
+      </c>
+      <c r="O24" t="s">
+        <v>22</v>
+      </c>
+      <c r="P24" t="n">
+        <v>85.871</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>79.66500000000001</v>
+      </c>
+      <c r="R24" t="n">
+        <v>83.29600000000001</v>
+      </c>
+      <c r="S24" t="s">
+        <v>21</v>
+      </c>
+      <c r="T24" t="s">
+        <v>23</v>
+      </c>
+      <c r="U24" t="n">
+        <v>85.07899999999999</v>
+      </c>
+      <c r="V24" t="n">
+        <v>58.596</v>
+      </c>
+      <c r="W24" t="n">
+        <v>72.10899999999999</v>
+      </c>
+      <c r="X24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row spans="1:24" r="25">
+      <c s="1" r="A25" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" t="n">
+        <v>194.3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" t="n">
+        <v>200.348</v>
+      </c>
+      <c r="G25" t="n">
+        <v>184.519</v>
+      </c>
+      <c r="H25" t="n">
+        <v>192.235</v>
+      </c>
+      <c r="I25" t="s">
+        <v>21</v>
+      </c>
+      <c r="J25" t="s">
+        <v>63</v>
+      </c>
+      <c r="K25" t="n">
+        <v>200.348</v>
+      </c>
+      <c r="L25" t="n">
+        <v>184.519</v>
+      </c>
+      <c r="M25" t="n">
+        <v>192.235</v>
+      </c>
+      <c r="N25" t="s">
+        <v>21</v>
+      </c>
+      <c r="O25" t="s">
+        <v>22</v>
+      </c>
+      <c r="P25" t="n">
+        <v>203.341</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>183.095</v>
+      </c>
+      <c r="R25" t="n">
+        <v>193.944</v>
+      </c>
+      <c r="S25" t="s">
+        <v>21</v>
+      </c>
+      <c r="T25" t="s">
+        <v>23</v>
+      </c>
+      <c r="U25" t="n">
+        <v>205.501</v>
+      </c>
+      <c r="V25" t="n">
+        <v>121.219</v>
+      </c>
+      <c r="W25" t="n">
+        <v>164.378</v>
+      </c>
+      <c r="X25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row spans="1:24" r="26">
+      <c s="1" r="A26" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" t="n">
+        <v>58.95</v>
+      </c>
+      <c r="E26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" t="n">
+        <v>57.999</v>
+      </c>
+      <c r="G26" t="n">
+        <v>53.351</v>
+      </c>
+      <c r="H26" t="n">
+        <v>55.731</v>
+      </c>
+      <c r="I26" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" t="s">
+        <v>63</v>
+      </c>
+      <c r="K26" t="n">
+        <v>57.999</v>
+      </c>
+      <c r="L26" t="n">
+        <v>53.351</v>
+      </c>
+      <c r="M26" t="n">
+        <v>55.731</v>
+      </c>
+      <c r="N26" t="s">
+        <v>21</v>
+      </c>
+      <c r="O26" t="s">
+        <v>22</v>
+      </c>
+      <c r="P26" t="n">
+        <v>59.008</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>53.793</v>
+      </c>
+      <c r="R26" t="n">
+        <v>57.853</v>
+      </c>
+      <c r="S26" t="s">
+        <v>25</v>
+      </c>
+      <c r="T26" t="s">
+        <v>23</v>
+      </c>
+      <c r="U26" t="n">
+        <v>60.795</v>
+      </c>
+      <c r="V26" t="n">
+        <v>51.224</v>
+      </c>
+      <c r="W26" t="n">
+        <v>55.448</v>
+      </c>
+      <c r="X26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row spans="1:24" r="27">
+      <c s="1" r="A27" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" t="n">
+        <v>4.07</v>
+      </c>
+      <c r="E27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" t="n">
+        <v>4.049</v>
+      </c>
+      <c r="G27" t="n">
+        <v>3.765</v>
+      </c>
+      <c r="H27" t="n">
+        <v>4.046</v>
+      </c>
+      <c r="I27" t="s">
+        <v>25</v>
+      </c>
+      <c r="J27" t="s">
+        <v>63</v>
+      </c>
+      <c r="K27" t="n">
+        <v>4.049</v>
+      </c>
+      <c r="L27" t="n">
+        <v>3.765</v>
+      </c>
+      <c r="M27" t="n">
+        <v>4.046</v>
+      </c>
+      <c r="N27" t="s">
+        <v>25</v>
+      </c>
+      <c r="O27" t="s">
+        <v>22</v>
+      </c>
+      <c r="P27" t="n">
+        <v>4.027</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>4.355</v>
+      </c>
+      <c r="R27" t="n">
+        <v>4.088</v>
+      </c>
+      <c r="S27" t="s">
+        <v>25</v>
+      </c>
+      <c r="T27" t="s">
+        <v>23</v>
+      </c>
+      <c r="U27" t="n">
+        <v>4.624</v>
+      </c>
+      <c r="V27" t="n">
+        <v>2.787</v>
+      </c>
+      <c r="W27" t="n">
+        <v>4.236</v>
+      </c>
+      <c r="X27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="28">
+      <c s="1" r="A28" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" t="n">
+        <v>357.55</v>
+      </c>
+      <c r="E28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" t="n">
+        <v>354.534</v>
+      </c>
+      <c r="G28" t="n">
+        <v>291.549</v>
+      </c>
+      <c r="H28" t="n">
+        <v>328.361</v>
+      </c>
+      <c r="I28" t="s">
+        <v>21</v>
+      </c>
+      <c r="J28" t="s">
+        <v>63</v>
+      </c>
+      <c r="K28" t="n">
+        <v>354.534</v>
+      </c>
+      <c r="L28" t="n">
+        <v>291.549</v>
+      </c>
+      <c r="M28" t="n">
+        <v>328.361</v>
+      </c>
+      <c r="N28" t="s">
+        <v>21</v>
+      </c>
+      <c r="O28" t="s">
+        <v>22</v>
+      </c>
+      <c r="P28" t="n">
+        <v>370.93</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>264.956</v>
+      </c>
+      <c r="R28" t="n">
+        <v>343.166</v>
+      </c>
+      <c r="S28" t="s">
+        <v>25</v>
+      </c>
+      <c r="T28" t="s">
+        <v>23</v>
+      </c>
+      <c r="U28" t="n">
+        <v>377.953</v>
+      </c>
+      <c r="V28" t="n">
+        <v>245.694</v>
+      </c>
+      <c r="W28" t="n">
+        <v>320.379</v>
+      </c>
+      <c r="X28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row spans="1:24" r="29">
+      <c s="1" r="A29" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" t="n">
+        <v>213.05</v>
+      </c>
+      <c r="E29" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" t="n">
+        <v>220.32</v>
+      </c>
+      <c r="G29" t="n">
+        <v>202.977</v>
+      </c>
+      <c r="H29" t="n">
+        <v>213.138</v>
+      </c>
+      <c r="I29" t="s">
+        <v>21</v>
+      </c>
+      <c r="J29" t="s">
+        <v>63</v>
+      </c>
+      <c r="K29" t="n">
+        <v>220.32</v>
+      </c>
+      <c r="L29" t="n">
+        <v>202.977</v>
+      </c>
+      <c r="M29" t="n">
+        <v>213.138</v>
+      </c>
+      <c r="N29" t="s">
+        <v>21</v>
+      </c>
+      <c r="O29" t="s">
+        <v>22</v>
+      </c>
+      <c r="P29" t="n">
+        <v>229.324</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>193.556</v>
+      </c>
+      <c r="R29" t="n">
+        <v>210.65</v>
+      </c>
+      <c r="S29" t="s">
+        <v>21</v>
+      </c>
+      <c r="T29" t="s">
+        <v>23</v>
+      </c>
+      <c r="U29" t="n">
+        <v>219.481</v>
+      </c>
+      <c r="V29" t="n">
+        <v>141.002</v>
+      </c>
+      <c r="W29" t="n">
+        <v>194.343</v>
+      </c>
+      <c r="X29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="30">
+      <c s="1" r="A30" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" t="n">
+        <v>17.215</v>
+      </c>
+      <c r="E30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" t="n">
+        <v>18.226</v>
+      </c>
+      <c r="G30" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="H30" t="n">
+        <v>16.323</v>
+      </c>
+      <c r="I30" t="s">
+        <v>21</v>
+      </c>
+      <c r="J30" t="s">
+        <v>63</v>
+      </c>
+      <c r="K30" t="n">
+        <v>18.226</v>
+      </c>
+      <c r="L30" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="M30" t="n">
+        <v>16.323</v>
+      </c>
+      <c r="N30" t="s">
+        <v>21</v>
+      </c>
+      <c r="O30" t="s">
+        <v>22</v>
+      </c>
+      <c r="P30" t="n">
+        <v>18.247</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>10.694</v>
+      </c>
+      <c r="R30" t="n">
+        <v>17.003</v>
+      </c>
+      <c r="S30" t="s">
+        <v>25</v>
+      </c>
+      <c r="T30" t="s">
+        <v>23</v>
+      </c>
+      <c r="U30" t="n">
+        <v>18.247</v>
+      </c>
+      <c r="V30" t="n">
+        <v>10.694</v>
+      </c>
+      <c r="W30" t="n">
+        <v>17.003</v>
+      </c>
+      <c r="X30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="31">
+      <c s="1" r="A31" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D31" t="n">
+        <v>76.905</v>
+      </c>
+      <c r="E31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" t="n">
+        <v>78.03700000000001</v>
+      </c>
+      <c r="G31" t="n">
+        <v>69.767</v>
+      </c>
+      <c r="H31" t="n">
+        <v>75.34399999999999</v>
+      </c>
+      <c r="I31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J31" t="s">
+        <v>63</v>
+      </c>
+      <c r="K31" t="n">
+        <v>78.03700000000001</v>
+      </c>
+      <c r="L31" t="n">
+        <v>69.767</v>
+      </c>
+      <c r="M31" t="n">
+        <v>75.34399999999999</v>
+      </c>
+      <c r="N31" t="s">
+        <v>25</v>
+      </c>
+      <c r="O31" t="s">
+        <v>22</v>
+      </c>
+      <c r="P31" t="n">
+        <v>80.18000000000001</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>68.855</v>
+      </c>
+      <c r="R31" t="n">
+        <v>74.81399999999999</v>
+      </c>
+      <c r="S31" t="s">
+        <v>21</v>
+      </c>
+      <c r="T31" t="s">
+        <v>23</v>
+      </c>
+      <c r="U31" t="n">
+        <v>77.298</v>
+      </c>
+      <c r="V31" t="n">
+        <v>54.366</v>
+      </c>
+      <c r="W31" t="n">
+        <v>69.553</v>
+      </c>
+      <c r="X31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row spans="1:24" r="32">
+      <c s="1" r="A32" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" t="n">
+        <v>66.47499999999999</v>
+      </c>
+      <c r="E32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" t="n">
+        <v>67.44499999999999</v>
+      </c>
+      <c r="G32" t="n">
+        <v>64.465</v>
+      </c>
+      <c r="H32" t="n">
+        <v>66.178</v>
+      </c>
+      <c r="I32" t="s">
+        <v>21</v>
+      </c>
+      <c r="J32" t="s">
+        <v>63</v>
+      </c>
+      <c r="K32" t="n">
+        <v>67.44499999999999</v>
+      </c>
+      <c r="L32" t="n">
+        <v>64.465</v>
+      </c>
+      <c r="M32" t="n">
+        <v>66.178</v>
+      </c>
+      <c r="N32" t="s">
+        <v>21</v>
+      </c>
+      <c r="O32" t="s">
+        <v>22</v>
+      </c>
+      <c r="P32" t="n">
+        <v>68.925</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>60.208</v>
+      </c>
+      <c r="R32" t="n">
+        <v>66.614</v>
+      </c>
+      <c r="S32" t="s">
+        <v>25</v>
+      </c>
+      <c r="T32" t="s">
+        <v>23</v>
+      </c>
+      <c r="U32" t="n">
+        <v>69.235</v>
+      </c>
+      <c r="V32" t="n">
+        <v>52.961</v>
+      </c>
+      <c r="W32" t="n">
+        <v>63.207</v>
+      </c>
+      <c r="X32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row spans="1:24" r="33">
+      <c s="1" r="A33" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" t="n">
+        <v>22.39</v>
+      </c>
+      <c r="E33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" t="n">
+        <v>28.961</v>
+      </c>
+      <c r="G33" t="n">
+        <v>20.828</v>
+      </c>
+      <c r="H33" t="n">
+        <v>27.288</v>
+      </c>
+      <c r="I33" t="s">
+        <v>25</v>
+      </c>
+      <c r="J33" t="s">
+        <v>63</v>
+      </c>
+      <c r="K33" t="n">
+        <v>28.961</v>
+      </c>
+      <c r="L33" t="n">
+        <v>20.828</v>
+      </c>
+      <c r="M33" t="n">
+        <v>27.288</v>
+      </c>
+      <c r="N33" t="s">
+        <v>25</v>
+      </c>
+      <c r="O33" t="s">
+        <v>22</v>
+      </c>
+      <c r="P33" t="n">
+        <v>30.246</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>19.006</v>
+      </c>
+      <c r="R33" t="n">
+        <v>27.251</v>
+      </c>
+      <c r="S33" t="s">
+        <v>25</v>
+      </c>
+      <c r="T33" t="s">
+        <v>23</v>
+      </c>
+      <c r="U33" t="n">
+        <v>30.246</v>
+      </c>
+      <c r="V33" t="n">
+        <v>19.006</v>
+      </c>
+      <c r="W33" t="n">
+        <v>27.251</v>
+      </c>
+      <c r="X33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="34">
+      <c s="1" r="A34" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" t="n">
+        <v>16.82</v>
+      </c>
+      <c r="E34" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" t="n">
+        <v>18.189</v>
+      </c>
+      <c r="G34" t="n">
+        <v>15.384</v>
+      </c>
+      <c r="H34" t="n">
+        <v>17.242</v>
+      </c>
+      <c r="I34" t="s">
+        <v>21</v>
+      </c>
+      <c r="J34" t="s">
+        <v>63</v>
+      </c>
+      <c r="K34" t="n">
+        <v>18.189</v>
+      </c>
+      <c r="L34" t="n">
+        <v>15.384</v>
+      </c>
+      <c r="M34" t="n">
+        <v>17.242</v>
+      </c>
+      <c r="N34" t="s">
+        <v>21</v>
+      </c>
+      <c r="O34" t="s">
+        <v>22</v>
+      </c>
+      <c r="P34" t="n">
+        <v>19.21</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>14.506</v>
+      </c>
+      <c r="R34" t="n">
+        <v>16.965</v>
+      </c>
+      <c r="S34" t="s">
+        <v>21</v>
+      </c>
+      <c r="T34" t="s">
+        <v>23</v>
+      </c>
+      <c r="U34" t="n">
+        <v>19.21</v>
+      </c>
+      <c r="V34" t="n">
+        <v>14.506</v>
+      </c>
+      <c r="W34" t="n">
+        <v>16.965</v>
+      </c>
+      <c r="X34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row spans="1:24" r="35">
+      <c s="1" r="A35" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" t="n">
+        <v>109.375</v>
+      </c>
+      <c r="E35" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" t="n">
+        <v>115.121</v>
+      </c>
+      <c r="G35" t="n">
+        <v>108.385</v>
+      </c>
+      <c r="H35" t="n">
+        <v>109.376</v>
+      </c>
+      <c r="I35" t="s">
+        <v>36</v>
+      </c>
+      <c r="J35" t="s">
+        <v>63</v>
+      </c>
+      <c r="K35" t="n">
+        <v>115.121</v>
+      </c>
+      <c r="L35" t="n">
+        <v>108.385</v>
+      </c>
+      <c r="M35" t="n">
+        <v>109.376</v>
+      </c>
+      <c r="N35" t="s">
+        <v>36</v>
+      </c>
+      <c r="O35" t="s">
+        <v>22</v>
+      </c>
+      <c r="P35" t="n">
+        <v>122.99</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>107.237</v>
+      </c>
+      <c r="R35" t="n">
+        <v>119.298</v>
+      </c>
+      <c r="S35" t="s">
+        <v>25</v>
+      </c>
+      <c r="T35" t="s">
+        <v>23</v>
+      </c>
+      <c r="U35" t="n">
+        <v>118.015</v>
+      </c>
+      <c r="V35" t="n">
+        <v>87.258</v>
+      </c>
+      <c r="W35" t="n">
+        <v>108.96</v>
+      </c>
+      <c r="X35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="36">
+      <c s="1" r="A36" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" t="n">
+        <v>9.904999999999999</v>
+      </c>
+      <c r="E36" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" t="n">
+        <v>11.262</v>
+      </c>
+      <c r="G36" t="n">
+        <v>9.651999999999999</v>
+      </c>
+      <c r="H36" t="n">
+        <v>10.994</v>
+      </c>
+      <c r="I36" t="s">
+        <v>25</v>
+      </c>
+      <c r="J36" t="s">
+        <v>63</v>
+      </c>
+      <c r="K36" t="n">
+        <v>11.262</v>
+      </c>
+      <c r="L36" t="n">
+        <v>9.651999999999999</v>
+      </c>
+      <c r="M36" t="n">
+        <v>10.994</v>
+      </c>
+      <c r="N36" t="s">
+        <v>25</v>
+      </c>
+      <c r="O36" t="s">
+        <v>22</v>
+      </c>
+      <c r="P36" t="n">
+        <v>10.826</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>7.595</v>
+      </c>
+      <c r="R36" t="n">
+        <v>10.49</v>
+      </c>
+      <c r="S36" t="s">
+        <v>25</v>
+      </c>
+      <c r="T36" t="s">
+        <v>23</v>
+      </c>
+      <c r="U36" t="n">
+        <v>10.826</v>
+      </c>
+      <c r="V36" t="n">
+        <v>7.595</v>
+      </c>
+      <c r="W36" t="n">
+        <v>10.49</v>
+      </c>
+      <c r="X36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="37">
+      <c s="1" r="A37" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" t="n">
+        <v>4.96</v>
+      </c>
+      <c r="E37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" t="n">
+        <v>4.916</v>
+      </c>
+      <c r="G37" t="n">
+        <v>4.187</v>
+      </c>
+      <c r="H37" t="n">
+        <v>4.66</v>
+      </c>
+      <c r="I37" t="s">
+        <v>21</v>
+      </c>
+      <c r="J37" t="s">
+        <v>63</v>
+      </c>
+      <c r="K37" t="n">
+        <v>4.916</v>
+      </c>
+      <c r="L37" t="n">
+        <v>4.187</v>
+      </c>
+      <c r="M37" t="n">
+        <v>4.66</v>
+      </c>
+      <c r="N37" t="s">
+        <v>21</v>
+      </c>
+      <c r="O37" t="s">
+        <v>22</v>
+      </c>
+      <c r="P37" t="n">
+        <v>5.955</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="R37" t="n">
+        <v>5.715</v>
+      </c>
+      <c r="S37" t="s">
+        <v>25</v>
+      </c>
+      <c r="T37" t="s">
+        <v>23</v>
+      </c>
+      <c r="U37" t="n">
+        <v>5.955</v>
+      </c>
+      <c r="V37" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="W37" t="n">
+        <v>5.715</v>
+      </c>
+      <c r="X37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="38">
+      <c s="1" r="A38" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" t="n">
+        <v>107.74</v>
+      </c>
+      <c r="E38" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" t="n">
+        <v>123.011</v>
+      </c>
+      <c r="G38" t="n">
+        <v>89.783</v>
+      </c>
+      <c r="H38" t="n">
+        <v>108.201</v>
+      </c>
+      <c r="I38" t="s">
+        <v>21</v>
+      </c>
+      <c r="J38" t="s">
+        <v>63</v>
+      </c>
+      <c r="K38" t="n">
+        <v>123.011</v>
+      </c>
+      <c r="L38" t="n">
+        <v>89.783</v>
+      </c>
+      <c r="M38" t="n">
+        <v>108.201</v>
+      </c>
+      <c r="N38" t="s">
+        <v>21</v>
+      </c>
+      <c r="O38" t="s">
+        <v>22</v>
+      </c>
+      <c r="P38" t="n">
+        <v>124.464</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>81.068</v>
+      </c>
+      <c r="R38" t="n">
+        <v>113.237</v>
+      </c>
+      <c r="S38" t="s">
+        <v>25</v>
+      </c>
+      <c r="T38" t="s">
+        <v>23</v>
+      </c>
+      <c r="U38" t="n">
+        <v>124.464</v>
+      </c>
+      <c r="V38" t="n">
+        <v>81.068</v>
+      </c>
+      <c r="W38" t="n">
+        <v>113.237</v>
+      </c>
+      <c r="X38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="39">
+      <c s="1" r="A39" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" t="n">
+        <v>12.76</v>
+      </c>
+      <c r="E39" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" t="n">
+        <v>15.566</v>
+      </c>
+      <c r="G39" t="n">
+        <v>12.597</v>
+      </c>
+      <c r="H39" t="n">
+        <v>14.403</v>
+      </c>
+      <c r="I39" t="s">
+        <v>21</v>
+      </c>
+      <c r="J39" t="s">
+        <v>63</v>
+      </c>
+      <c r="K39" t="n">
+        <v>15.566</v>
+      </c>
+      <c r="L39" t="n">
+        <v>12.597</v>
+      </c>
+      <c r="M39" t="n">
+        <v>14.403</v>
+      </c>
+      <c r="N39" t="s">
+        <v>21</v>
+      </c>
+      <c r="O39" t="s">
+        <v>22</v>
+      </c>
+      <c r="P39" t="n">
+        <v>14.607</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>11.578</v>
+      </c>
+      <c r="R39" t="n">
+        <v>12.377</v>
+      </c>
+      <c r="S39" t="s">
+        <v>36</v>
+      </c>
+      <c r="T39" t="s">
+        <v>23</v>
+      </c>
+      <c r="U39" t="n">
+        <v>17.091</v>
+      </c>
+      <c r="V39" t="n">
+        <v>12.073</v>
+      </c>
+      <c r="W39" t="n">
+        <v>13.714</v>
+      </c>
+      <c r="X39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row spans="1:24" r="40">
+      <c s="1" r="A40" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" t="n">
+        <v>44.09</v>
+      </c>
+      <c r="E40" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" t="n">
+        <v>44.099</v>
+      </c>
+      <c r="G40" t="n">
+        <v>40.163</v>
+      </c>
+      <c r="H40" t="n">
+        <v>43.422</v>
+      </c>
+      <c r="I40" t="s">
+        <v>25</v>
+      </c>
+      <c r="J40" t="s">
+        <v>63</v>
+      </c>
+      <c r="K40" t="n">
+        <v>44.099</v>
+      </c>
+      <c r="L40" t="n">
+        <v>40.163</v>
+      </c>
+      <c r="M40" t="n">
+        <v>43.422</v>
+      </c>
+      <c r="N40" t="s">
+        <v>25</v>
+      </c>
+      <c r="O40" t="s">
+        <v>22</v>
+      </c>
+      <c r="P40" t="n">
+        <v>44.906</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>38.783</v>
+      </c>
+      <c r="R40" t="n">
+        <v>44.723</v>
+      </c>
+      <c r="S40" t="s">
+        <v>25</v>
+      </c>
+      <c r="T40" t="s">
+        <v>23</v>
+      </c>
+      <c r="U40" t="n">
+        <v>44.778</v>
+      </c>
+      <c r="V40" t="n">
+        <v>31.739</v>
+      </c>
+      <c r="W40" t="n">
+        <v>40.72</v>
+      </c>
+      <c r="X40" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="41">
+      <c s="1" r="A41" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" t="s">
+        <v>29</v>
+      </c>
+      <c r="D41" t="n">
+        <v>319.91</v>
+      </c>
+      <c r="E41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" t="n">
+        <v>331.861</v>
+      </c>
+      <c r="G41" t="n">
+        <v>297.433</v>
+      </c>
+      <c r="H41" t="n">
+        <v>320.321</v>
+      </c>
+      <c r="I41" t="s">
+        <v>21</v>
+      </c>
+      <c r="J41" t="s">
+        <v>63</v>
+      </c>
+      <c r="K41" t="n">
+        <v>331.861</v>
+      </c>
+      <c r="L41" t="n">
+        <v>297.433</v>
+      </c>
+      <c r="M41" t="n">
+        <v>320.321</v>
+      </c>
+      <c r="N41" t="s">
+        <v>21</v>
+      </c>
+      <c r="O41" t="s">
+        <v>22</v>
+      </c>
+      <c r="P41" t="n">
+        <v>337.589</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>289.76</v>
+      </c>
+      <c r="R41" t="n">
+        <v>316.664</v>
+      </c>
+      <c r="S41" t="s">
+        <v>21</v>
+      </c>
+      <c r="T41" t="s">
+        <v>23</v>
+      </c>
+      <c r="U41" t="n">
+        <v>370.85</v>
+      </c>
+      <c r="V41" t="n">
+        <v>245.112</v>
+      </c>
+      <c r="W41" t="n">
+        <v>312.174</v>
+      </c>
+      <c r="X41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row spans="1:24" r="42">
+      <c s="1" r="A42" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" t="n">
+        <v>20.52</v>
+      </c>
+      <c r="E42" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" t="n">
+        <v>22.143</v>
+      </c>
+      <c r="G42" t="n">
+        <v>19.797</v>
+      </c>
+      <c r="H42" t="n">
+        <v>21.697</v>
+      </c>
+      <c r="I42" t="s">
+        <v>25</v>
+      </c>
+      <c r="J42" t="s">
+        <v>63</v>
+      </c>
+      <c r="K42" t="n">
+        <v>22.143</v>
+      </c>
+      <c r="L42" t="n">
+        <v>19.797</v>
+      </c>
+      <c r="M42" t="n">
+        <v>21.697</v>
+      </c>
+      <c r="N42" t="s">
+        <v>25</v>
+      </c>
+      <c r="O42" t="s">
+        <v>22</v>
+      </c>
+      <c r="P42" t="n">
+        <v>23.753</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>18.509</v>
+      </c>
+      <c r="R42" t="n">
+        <v>22.688</v>
+      </c>
+      <c r="S42" t="s">
+        <v>25</v>
+      </c>
+      <c r="T42" t="s">
+        <v>23</v>
+      </c>
+      <c r="U42" t="n">
+        <v>24.417</v>
+      </c>
+      <c r="V42" t="n">
+        <v>15.561</v>
+      </c>
+      <c r="W42" t="n">
+        <v>21.729</v>
+      </c>
+      <c r="X42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="43">
+      <c s="1" r="A43" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" t="n">
+        <v>9.84</v>
+      </c>
+      <c r="E43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" t="n">
+        <v>9.84</v>
+      </c>
+      <c r="G43" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="H43" t="n">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="I43" t="s">
+        <v>25</v>
+      </c>
+      <c r="J43" t="s">
+        <v>63</v>
+      </c>
+      <c r="K43" t="n">
+        <v>9.84</v>
+      </c>
+      <c r="L43" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="M43" t="n">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="N43" t="s">
+        <v>25</v>
+      </c>
+      <c r="O43" t="s">
+        <v>22</v>
+      </c>
+      <c r="P43" t="n">
+        <v>10.085</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>8.869999999999999</v>
+      </c>
+      <c r="R43" t="n">
+        <v>9.872999999999999</v>
+      </c>
+      <c r="S43" t="s">
+        <v>25</v>
+      </c>
+      <c r="T43" t="s">
+        <v>23</v>
+      </c>
+      <c r="U43" t="n">
+        <v>11.599</v>
+      </c>
+      <c r="V43" t="n">
+        <v>8.143000000000001</v>
+      </c>
+      <c r="W43" t="n">
+        <v>10.543</v>
+      </c>
+      <c r="X43" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="44">
+      <c s="1" r="A44" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" t="n">
+        <v>14.525</v>
+      </c>
+      <c r="E44" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" t="n">
+        <v>15.315</v>
+      </c>
+      <c r="G44" t="n">
+        <v>13.074</v>
+      </c>
+      <c r="H44" t="n">
+        <v>14.807</v>
+      </c>
+      <c r="I44" t="s">
+        <v>25</v>
+      </c>
+      <c r="J44" t="s">
+        <v>63</v>
+      </c>
+      <c r="K44" t="n">
+        <v>15.315</v>
+      </c>
+      <c r="L44" t="n">
+        <v>13.074</v>
+      </c>
+      <c r="M44" t="n">
+        <v>14.807</v>
+      </c>
+      <c r="N44" t="s">
+        <v>25</v>
+      </c>
+      <c r="O44" t="s">
+        <v>22</v>
+      </c>
+      <c r="P44" t="n">
+        <v>15.983</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>13.352</v>
+      </c>
+      <c r="R44" t="n">
+        <v>15.506</v>
+      </c>
+      <c r="S44" t="s">
+        <v>25</v>
+      </c>
+      <c r="T44" t="s">
+        <v>23</v>
+      </c>
+      <c r="U44" t="n">
+        <v>25.949</v>
+      </c>
+      <c r="V44" t="n">
+        <v>12.367</v>
+      </c>
+      <c r="W44" t="n">
+        <v>20.381</v>
+      </c>
+      <c r="X44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row spans="1:24" r="45">
+      <c s="1" r="A45" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" t="n">
+        <v>116.425</v>
+      </c>
+      <c r="E45" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" t="n">
+        <v>116.167</v>
+      </c>
+      <c r="G45" t="n">
+        <v>105.919</v>
+      </c>
+      <c r="H45" t="n">
+        <v>112.982</v>
+      </c>
+      <c r="I45" t="s">
+        <v>25</v>
+      </c>
+      <c r="J45" t="s">
+        <v>63</v>
+      </c>
+      <c r="K45" t="n">
+        <v>116.167</v>
+      </c>
+      <c r="L45" t="n">
+        <v>105.919</v>
+      </c>
+      <c r="M45" t="n">
+        <v>112.982</v>
+      </c>
+      <c r="N45" t="s">
+        <v>25</v>
+      </c>
+      <c r="O45" t="s">
+        <v>22</v>
+      </c>
+      <c r="P45" t="n">
+        <v>112.359</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>95.434</v>
+      </c>
+      <c r="R45" t="n">
+        <v>110.183</v>
+      </c>
+      <c r="S45" t="s">
+        <v>25</v>
+      </c>
+      <c r="T45" t="s">
+        <v>23</v>
+      </c>
+      <c r="U45" t="n">
+        <v>118.648</v>
+      </c>
+      <c r="V45" t="n">
+        <v>64.896</v>
+      </c>
+      <c r="W45" t="n">
+        <v>96.974</v>
+      </c>
+      <c r="X45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row spans="1:24" r="46">
+      <c s="1" r="A46" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" t="s">
+        <v>42</v>
+      </c>
+      <c r="D46" t="n">
+        <v>72.295</v>
+      </c>
+      <c r="E46" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" t="n">
+        <v>74.158</v>
+      </c>
+      <c r="G46" t="n">
+        <v>68.142</v>
+      </c>
+      <c r="H46" t="n">
+        <v>71.934</v>
+      </c>
+      <c r="I46" t="s">
+        <v>21</v>
+      </c>
+      <c r="J46" t="s">
+        <v>63</v>
+      </c>
+      <c r="K46" t="n">
+        <v>74.158</v>
+      </c>
+      <c r="L46" t="n">
+        <v>68.142</v>
+      </c>
+      <c r="M46" t="n">
+        <v>71.934</v>
+      </c>
+      <c r="N46" t="s">
+        <v>21</v>
+      </c>
+      <c r="O46" t="s">
+        <v>22</v>
+      </c>
+      <c r="P46" t="n">
+        <v>87.10599999999999</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>66.351</v>
+      </c>
+      <c r="R46" t="n">
+        <v>76.304</v>
+      </c>
+      <c r="S46" t="s">
+        <v>21</v>
+      </c>
+      <c r="T46" t="s">
+        <v>23</v>
+      </c>
+      <c r="U46" t="n">
+        <v>75.974</v>
+      </c>
+      <c r="V46" t="n">
+        <v>54.21</v>
+      </c>
+      <c r="W46" t="n">
+        <v>72.547</v>
+      </c>
+      <c r="X46" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="47">
+      <c s="1" r="A47" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" t="n">
+        <v>46.335</v>
+      </c>
+      <c r="E47" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" t="n">
+        <v>49.148</v>
+      </c>
+      <c r="G47" t="n">
+        <v>44.835</v>
+      </c>
+      <c r="H47" t="n">
+        <v>46.505</v>
+      </c>
+      <c r="I47" t="s">
+        <v>21</v>
+      </c>
+      <c r="J47" t="s">
+        <v>63</v>
+      </c>
+      <c r="K47" t="n">
+        <v>49.148</v>
+      </c>
+      <c r="L47" t="n">
+        <v>44.835</v>
+      </c>
+      <c r="M47" t="n">
+        <v>46.505</v>
+      </c>
+      <c r="N47" t="s">
+        <v>21</v>
+      </c>
+      <c r="O47" t="s">
+        <v>22</v>
+      </c>
+      <c r="P47" t="n">
+        <v>48.575</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>42.655</v>
+      </c>
+      <c r="R47" t="n">
+        <v>44.101</v>
+      </c>
+      <c r="S47" t="s">
+        <v>36</v>
+      </c>
+      <c r="T47" t="s">
+        <v>23</v>
+      </c>
+      <c r="U47" t="n">
+        <v>48.819</v>
+      </c>
+      <c r="V47" t="n">
+        <v>27.869</v>
+      </c>
+      <c r="W47" t="n">
+        <v>43.819</v>
+      </c>
+      <c r="X47" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row spans="1:24" r="48">
+      <c s="1" r="A48" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>79</v>
       </c>
       <c r="C48" t="s">
         <v>78</v>

</xml_diff>